<commit_message>
Fix Test cases 1
</commit_message>
<xml_diff>
--- a/FileBaoCao/CTS6326_Test cases.xlsx
+++ b/FileBaoCao/CTS6326_Test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCHOOL\NAM5-HK1\PTTKDBCL-KTLTHDT\Electronic_Components_Website\FileBaoCao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F1C7FE-F8D9-498D-A10D-AAB35E3787FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD27F2E-3E95-46FB-AFD8-727A272CB4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="92">
   <si>
     <t>Thiết kế</t>
   </si>
@@ -127,7 +127,175 @@
     <t>Thêm sản phẩm vào giỏ hàng</t>
   </si>
   <si>
-    <t>Chọn sản phẩm muốn thêm</t>
+    <t>Chọn sản phẩm</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>Điều chỉnh số lượng</t>
+  </si>
+  <si>
+    <t>Hiển thị thông tin sản phẩm chọn</t>
+  </si>
+  <si>
+    <t>Thay đổi số lượng muốn thêm vào giỏ hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thông báo lỗi </t>
+  </si>
+  <si>
+    <t>Chưa đăng nhập tài khoản</t>
+  </si>
+  <si>
+    <t>Thêm sản phẩm thành công</t>
+  </si>
+  <si>
+    <t>Thông báo thành công</t>
+  </si>
+  <si>
+    <t>Cập nhật số lượng sản phẩm trong giỏ hàng</t>
+  </si>
+  <si>
+    <t>Điều chỉnh số lượng tăng giảm</t>
+  </si>
+  <si>
+    <t>Thông báo thay đổi</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>Xóa sản phẩm trong giỏ hàng</t>
+  </si>
+  <si>
+    <t>Xóa sản phẩm</t>
+  </si>
+  <si>
+    <t>Đặt hàng</t>
+  </si>
+  <si>
+    <t>Chọn đặt hàng trong giỏ hàng</t>
+  </si>
+  <si>
+    <t>Hiển thị giao diện đặt hàng</t>
+  </si>
+  <si>
+    <t>yêu cầu nhập, chọn</t>
+  </si>
+  <si>
+    <t>Các trường liên quan</t>
+  </si>
+  <si>
+    <t>Các trường thông tin khách hàng</t>
+  </si>
+  <si>
+    <t>Tự động cập nhật thông tin lên các trường</t>
+  </si>
+  <si>
+    <t>(Nguyễn Xuân Thường, 97 Man thiện, 0987654321)</t>
+  </si>
+  <si>
+    <t>Đặt hàng thành công</t>
+  </si>
+  <si>
+    <t>Thông báo thành công, chuyển đến trang đặt hàng</t>
+  </si>
+  <si>
+    <t>Đặt hàng thất bại</t>
+  </si>
+  <si>
+    <t>Lỗi server</t>
+  </si>
+  <si>
+    <t>Thông báo lỗi</t>
+  </si>
+  <si>
+    <t>Hủy đơn hàng</t>
+  </si>
+  <si>
+    <t>Hủy thất bại</t>
+  </si>
+  <si>
+    <t>Thông báo đơn hủy thất bại</t>
+  </si>
+  <si>
+    <t>Hủy thành công</t>
+  </si>
+  <si>
+    <t>cột status không phải Chưa xác nhận hoặc Đã xác nhận</t>
+  </si>
+  <si>
+    <t>cột status là chưa xác nhận hoặc Đã xác nhận</t>
+  </si>
+  <si>
+    <t>Thay đổi thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>Thông báo thay đổi thành công</t>
+  </si>
+  <si>
+    <t>Thay đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Mật khẩu mới và mật khẩu xác nhận khác nhau</t>
+  </si>
+  <si>
+    <t>(123123, 123456)</t>
+  </si>
+  <si>
+    <t>Thông báo cụ thể mật khẩu không khớp</t>
+  </si>
+  <si>
+    <t>sai mật khẩu củ</t>
+  </si>
+  <si>
+    <t>(123123, 123456, 123456)</t>
+  </si>
+  <si>
+    <t>Thêm sản phẩm</t>
+  </si>
+  <si>
+    <t>Yêu cầu nhập, chọn</t>
+  </si>
+  <si>
+    <t>Dữ liệu nhập sai</t>
+  </si>
+  <si>
+    <t>Thêm đúng</t>
+  </si>
+  <si>
+    <t>Thay đổi đúng</t>
+  </si>
+  <si>
+    <t>(123123 != 123456)</t>
+  </si>
+  <si>
+    <t>Thông báo thêm thành công và trở về màn hình danh sách sản phẩm</t>
+  </si>
+  <si>
+    <t>Thêm nhân viên</t>
+  </si>
+  <si>
+    <t>Thay đổi thông tin nhân viên</t>
+  </si>
+  <si>
+    <t>Thay đổi trạng thái khách hàng</t>
+  </si>
+  <si>
+    <t>Thanh đổi thành công</t>
+  </si>
+  <si>
+    <t>Trạng thái hoạt động -&gt; khóa</t>
+  </si>
+  <si>
+    <t>Thêm đơn nhập</t>
   </si>
 </sst>
 </file>
@@ -197,7 +365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -220,17 +388,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -240,7 +397,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -267,21 +424,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -694,17 +856,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H27"/>
+  <dimension ref="B2:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="35.44140625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
@@ -842,7 +1004,7 @@
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -911,7 +1073,7 @@
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="14" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -932,6 +1094,7 @@
       <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
@@ -945,40 +1108,45 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14">
+      <c r="B19" s="10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="14">
+      <c r="B20" s="10">
         <v>4.2</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>33</v>
       </c>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19">
+      <c r="B21" s="10">
         <v>4.3</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
@@ -992,38 +1160,697 @@
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="19">
+      <c r="B23" s="10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="19">
+      <c r="B24" s="10">
         <v>5.2</v>
       </c>
+      <c r="C24" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="19">
+      <c r="B25" s="10">
         <v>5.3</v>
       </c>
+      <c r="C25" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="19">
+      <c r="B26" s="10">
         <v>5.4</v>
       </c>
+      <c r="C26" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="19">
+      <c r="B27" s="10">
         <v>5.4</v>
       </c>
+      <c r="C27" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="18">
+        <v>6.1</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="8">
+        <v>7</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="18">
+        <v>7.1</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="8">
+        <v>8</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="18">
+        <v>8.1</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="2:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="20">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="20"/>
+    </row>
+    <row r="35" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="20">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="20"/>
+    </row>
+    <row r="36" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="20">
+        <v>8.4</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="20"/>
+    </row>
+    <row r="37" spans="2:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="20">
+        <v>8.5</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="20"/>
+    </row>
+    <row r="38" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="20">
+        <v>8.6</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="20"/>
+    </row>
+    <row r="39" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="8">
+        <v>9</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="2:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="8">
+        <v>10</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="2:6" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
+        <v>10.3</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="8">
+        <v>11</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="2:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="8">
+        <v>12</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="8">
+        <v>13</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="2:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="3">
+        <v>13.4</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="8">
+        <v>14</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="8">
+        <v>15</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="E65" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="8">
+        <v>16</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="3"/>
+      <c r="E70" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="3">
+        <v>16.2</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D71" s="3"/>
+      <c r="E71" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="3">
+        <v>16.3</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D11" r:id="rId1" xr:uid="{47BC26E7-27AE-4D76-9A8E-E0B376187815}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="68" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>